<commit_message>
got the map to label my 77 district, and made pie chart of overall salary in Chicago
</commit_message>
<xml_diff>
--- a/areasalarys.xlsx
+++ b/areasalarys.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>area</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve"> lessthan25000</t>
+  </si>
+  <si>
+    <t>Chicago</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1097,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,10 +1130,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>300788</v>
@@ -1147,10 +1150,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
       <c r="C3">
         <v>15752</v>
@@ -1167,10 +1170,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
       <c r="C4">
         <v>12512</v>
@@ -1187,10 +1190,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
       <c r="C5">
         <v>22164</v>
@@ -1207,10 +1210,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
       </c>
       <c r="C6">
         <v>7258</v>
@@ -1227,10 +1230,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
       <c r="C7">
         <v>3852</v>
@@ -1247,10 +1250,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
       </c>
       <c r="C8">
         <v>17568</v>
@@ -1267,10 +1270,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
       </c>
       <c r="C9">
         <v>11624</v>
@@ -1287,10 +1290,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
       </c>
       <c r="C10">
         <v>19048</v>
@@ -1307,10 +1310,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
       </c>
       <c r="C11">
         <v>1370</v>
@@ -1327,10 +1330,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
       </c>
       <c r="C12">
         <v>5188</v>
@@ -1347,10 +1350,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
       </c>
       <c r="C13">
         <v>4058</v>
@@ -1367,10 +1370,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
       </c>
       <c r="C14">
         <v>1730</v>
@@ -1387,10 +1390,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
       </c>
       <c r="C15">
         <v>3672</v>
@@ -1407,10 +1410,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
       </c>
       <c r="C16">
         <v>9612</v>
@@ -1427,10 +1430,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
       </c>
       <c r="C17">
         <v>10018</v>
@@ -1447,10 +1450,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
       </c>
       <c r="C18">
         <v>8018</v>
@@ -1467,10 +1470,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
       </c>
       <c r="C19">
         <v>5968</v>
@@ -1487,10 +1490,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
       <c r="C20">
         <v>2306</v>
@@ -1507,10 +1510,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
       </c>
       <c r="C21">
         <v>12096</v>
@@ -1527,10 +1530,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
       </c>
       <c r="C22">
         <v>3576</v>
@@ -1547,10 +1550,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
       </c>
       <c r="C23">
         <v>6904</v>
@@ -1567,10 +1570,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
       </c>
       <c r="C24">
         <v>14526</v>
@@ -1587,10 +1590,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
       </c>
       <c r="C25">
         <v>14918</v>
@@ -1607,10 +1610,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
       </c>
       <c r="C26">
         <v>16656</v>
@@ -1627,10 +1630,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
       </c>
       <c r="C27">
         <v>26950</v>
@@ -1647,10 +1650,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
       </c>
       <c r="C28">
         <v>6410</v>
@@ -1667,10 +1670,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
       </c>
       <c r="C29">
         <v>6796</v>
@@ -1687,10 +1690,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
       </c>
       <c r="C30">
         <v>13896</v>
@@ -1707,10 +1710,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
       </c>
       <c r="C31">
         <v>10738</v>
@@ -1727,10 +1730,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
       </c>
       <c r="C32">
         <v>11688</v>
@@ -1747,10 +1750,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
       </c>
       <c r="C33">
         <v>8606</v>
@@ -1767,10 +1770,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
       </c>
       <c r="C34">
         <v>3636</v>
@@ -1787,10 +1790,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
         <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
       </c>
       <c r="C35">
         <v>4072</v>
@@ -1807,10 +1810,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
       </c>
       <c r="C36">
         <v>4866</v>
@@ -1827,10 +1830,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
       </c>
       <c r="C37">
         <v>7422</v>
@@ -1847,10 +1850,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
       </c>
       <c r="C38">
         <v>8964</v>
@@ -1867,10 +1870,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>39</v>
       </c>
       <c r="C39">
         <v>1416</v>
@@ -1887,10 +1890,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
       </c>
       <c r="C40">
         <v>8964</v>
@@ -1907,10 +1910,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
       </c>
       <c r="C41">
         <v>7034</v>
@@ -1927,10 +1930,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
         <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
       </c>
       <c r="C42">
         <v>4304</v>
@@ -1947,10 +1950,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
         <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>43</v>
       </c>
       <c r="C43">
         <v>8032</v>
@@ -1967,10 +1970,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
         <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>44</v>
       </c>
       <c r="C44">
         <v>9456</v>
@@ -1987,10 +1990,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
         <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>45</v>
       </c>
       <c r="C45">
         <v>20898</v>
@@ -2007,10 +2010,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
         <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>46</v>
       </c>
       <c r="C46">
         <v>12558</v>
@@ -2027,10 +2030,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
         <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>47</v>
       </c>
       <c r="C47">
         <v>2254</v>
@@ -2047,10 +2050,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
         <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>48</v>
       </c>
       <c r="C48">
         <v>9530</v>
@@ -2067,10 +2070,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
         <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>49</v>
       </c>
       <c r="C49">
         <v>1010</v>
@@ -2087,10 +2090,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
         <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
       </c>
       <c r="C50">
         <v>2442</v>
@@ -2107,10 +2110,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
         <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>51</v>
       </c>
       <c r="C51">
         <v>10870</v>
@@ -2127,10 +2130,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
         <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>52</v>
       </c>
       <c r="C52">
         <v>1974</v>
@@ -2147,10 +2150,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
         <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>53</v>
       </c>
       <c r="C53">
         <v>3978</v>
@@ -2167,10 +2170,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
         <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>54</v>
       </c>
       <c r="C54">
         <v>4186</v>
@@ -2187,10 +2190,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
         <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>55</v>
       </c>
       <c r="C55">
         <v>6756</v>
@@ -2207,10 +2210,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
         <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>56</v>
       </c>
       <c r="C56">
         <v>2768</v>
@@ -2227,10 +2230,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
         <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>57</v>
       </c>
       <c r="C57">
         <v>1822</v>
@@ -2247,10 +2250,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
         <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>58</v>
       </c>
       <c r="C58">
         <v>4590</v>
@@ -2267,10 +2270,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
         <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>59</v>
       </c>
       <c r="C59">
         <v>1556</v>
@@ -2287,10 +2290,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
         <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>60</v>
       </c>
       <c r="C60">
         <v>7276</v>
@@ -2307,10 +2310,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
         <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
       </c>
       <c r="C61">
         <v>2766</v>
@@ -2327,10 +2330,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>62</v>
       </c>
       <c r="C62">
         <v>7380</v>
@@ -2347,10 +2350,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
         <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>63</v>
       </c>
       <c r="C63">
         <v>9488</v>
@@ -2367,10 +2370,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
         <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>64</v>
       </c>
       <c r="C64">
         <v>1532</v>
@@ -2387,10 +2390,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
         <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>65</v>
       </c>
       <c r="C65">
         <v>4724</v>
@@ -2407,10 +2410,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
         <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>66</v>
       </c>
       <c r="C66">
         <v>3272</v>
@@ -2427,10 +2430,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
         <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>67</v>
       </c>
       <c r="C67">
         <v>4198</v>
@@ -2447,10 +2450,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
         <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>68</v>
       </c>
       <c r="C68">
         <v>9972</v>
@@ -2467,10 +2470,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
         <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>69</v>
       </c>
       <c r="C69">
         <v>10076</v>
@@ -2487,10 +2490,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
         <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>70</v>
       </c>
       <c r="C70">
         <v>12924</v>
@@ -2507,10 +2510,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
         <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>71</v>
       </c>
       <c r="C71">
         <v>12092</v>
@@ -2527,10 +2530,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
         <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>72</v>
       </c>
       <c r="C72">
         <v>3976</v>
@@ -2547,10 +2550,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
         <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>73</v>
       </c>
       <c r="C73">
         <v>13804</v>
@@ -2567,10 +2570,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
         <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>74</v>
       </c>
       <c r="C74">
         <v>1932</v>
@@ -2587,10 +2590,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
         <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>75</v>
       </c>
       <c r="C75">
         <v>5676</v>
@@ -2607,10 +2610,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
         <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>76</v>
       </c>
       <c r="C76">
         <v>1282</v>
@@ -2627,10 +2630,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
         <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>77</v>
       </c>
       <c r="C77">
         <v>3940</v>
@@ -2647,10 +2650,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
         <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>78</v>
       </c>
       <c r="C78">
         <v>2152</v>
@@ -2666,6 +2669,12 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
       <c r="C79">
         <v>18514</v>
       </c>

</xml_diff>